<commit_message>
add test cases for connector realtime
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-realtime-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-realtime-test-data.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20113AF1-ECD8-4296-A5D1-9B1D58849786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8194B1AE-4E5D-4A6D-9A9B-57D8779E4584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loadBundle" sheetId="1" r:id="rId1"/>
+    <sheet name="pluginOperation" sheetId="2" r:id="rId2"/>
+    <sheet name="getPluginInformation" sheetId="3" r:id="rId3"/>
+    <sheet name="pluginInstanceStart" sheetId="4" r:id="rId4"/>
+    <sheet name="pluginRunningLogInformation" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="78">
   <si>
     <t>test-id</t>
   </si>
@@ -45,12 +49,6 @@
     <t>200</t>
   </si>
   <si>
-    <t>100000</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>iot-connector-realtime-loadBundle-Test-1</t>
   </si>
   <si>
@@ -73,13 +71,230 @@
   </si>
   <si>
     <t>InKafka</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Operate success</t>
+  </si>
+  <si>
+    <t>pluginState</t>
+  </si>
+  <si>
+    <t>INIT</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-1</t>
+  </si>
+  <si>
+    <t>bad request,load plugin with the same file again</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-loadBundle-Test-2</t>
+  </si>
+  <si>
+    <t>106602</t>
+  </si>
+  <si>
+    <t>already loaded</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>pre-executionOfLoadBundle</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "file": "inKafkaPlugin-1.0-SNAPSHOT-all.zip"
+    }
+]</t>
+  </si>
+  <si>
+    <t>pre-executionOfPluginOperation</t>
+  </si>
+  <si>
+    <t>STARTED</t>
+  </si>
+  <si>
+    <t>good request,start "STOPPED" plugin</t>
+  </si>
+  <si>
+    <t>bad request,start plugin again</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "operator": "START",
+        "pluginId": "InKafkaTestPlugin"
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "operator": "STOP",
+        "pluginId": "InKafkaTestPlugin"
+    }
+]</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-2</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-3</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-4</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "operator": "UNLOAD",
+        "pluginId": "InKafkaTestPlugin"
+    }
+]</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-5</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-6</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-7</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-8</t>
+  </si>
+  <si>
+    <t>good request,stop "STARTED" plugin</t>
+  </si>
+  <si>
+    <t>bad request,stop plugin again</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-9</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-10</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-11</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginOperation-Test-12</t>
+  </si>
+  <si>
+    <t>good request,unload "STARTED" plugin</t>
+  </si>
+  <si>
+    <t>good request,unload "STOPPED" plugin</t>
+  </si>
+  <si>
+    <t>bad request,unload plugin again</t>
+  </si>
+  <si>
+    <t>UNLOAD</t>
+  </si>
+  <si>
+    <t>good request,start "INIT" plugin</t>
+  </si>
+  <si>
+    <t>good request,stop "INIT" plugin</t>
+  </si>
+  <si>
+    <t>good request,unload "INIT" plugin</t>
+  </si>
+  <si>
+    <t>bad request,start "UNLOADED" plugin</t>
+  </si>
+  <si>
+    <t>bad request,stop "UNLOADED" plugin</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-getPluginInformation-Test-1</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-getPluginInformation-Test-2</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-getPluginInformation-Test-3</t>
+  </si>
+  <si>
+    <t>good request, "INIT" plugin</t>
+  </si>
+  <si>
+    <t>good request, "STARTED" plugin</t>
+  </si>
+  <si>
+    <t>good request, "STOPPED" plugin</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-getPluginInformation-Test-4</t>
+  </si>
+  <si>
+    <t>bad request,plugin does not exist</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginInstanceStart-Test-1</t>
+  </si>
+  <si>
+    <t>good request, plugin is started</t>
+  </si>
+  <si>
+    <t>connectorName</t>
+  </si>
+  <si>
+    <t>locatorName</t>
+  </si>
+  <si>
+    <t>stopTime</t>
+  </si>
+  <si>
+    <t>locatorForRealtimePlugin</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>realtimePlugin</t>
+  </si>
+  <si>
+    <t>pre-executionOfPluginInstanceStart</t>
+  </si>
+  <si>
+    <t>iot-connector-realtime-pluginRunningLogInformation-Test-1</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "connectorName": "realtimePlugin",
+        "locatorName": "locatorForRealtimePlugin",
+        "stopTime":"10"
+    }
+]</t>
+  </si>
+  <si>
+    <t>600</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +305,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -160,6 +381,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -442,26 +672,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" style="6" customWidth="1"/>
     <col min="3" max="3" width="9.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.77734375" style="3"/>
+    <col min="5" max="5" width="39.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,48 +701,929 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="69" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C07D32A-ACF5-48EF-A7DA-25391FD309CD}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.77734375" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="69" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="69" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="9">
+        <v>106602</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="69" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="9">
+        <v>200</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="9">
+        <v>200</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="9">
+        <v>200</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="9">
+        <v>200</v>
+      </c>
+      <c r="I13" s="9">
+        <v>106602</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C85383F-AEE2-4241-9106-0D01144C8F6A}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="69" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905B0079-FCED-47EC-923E-5E704BBFD517}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.77734375" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>7</v>
+      <c r="K2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5828F07-1A21-4C10-995A-0FE7A8395A91}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>